<commit_message>
report are corrected till vertical scroll widget
</commit_message>
<xml_diff>
--- a/testData/widgetUrls.xlsx
+++ b/testData/widgetUrls.xlsx
@@ -1,44 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Playwright\Playwright-BDDCucumber-POM-15.01-External Testing\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A4EBE4-932F-47EC-B012-8FE629D54D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="URLs" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>WebsiteName</t>
+  </si>
+  <si>
+    <t>https://www.needingadvice.co.uk/</t>
+  </si>
+  <si>
+    <t>needingadvice_co_uk</t>
+  </si>
+  <si>
+    <t>https://plurality.network/</t>
+  </si>
+  <si>
+    <t>plurality_network</t>
+  </si>
+  <si>
+    <t>https://rateswitchrewards.co.uk/</t>
+  </si>
+  <si>
+    <t>rateswitchrewards_co_uk</t>
+  </si>
+  <si>
+    <t>http://samantus.com/</t>
+  </si>
+  <si>
+    <t>samantus_com</t>
+  </si>
+  <si>
+    <t>https://www.schoolofpodcasting.com/</t>
+  </si>
+  <si>
+    <t>schoolofpodcasting_com</t>
+  </si>
+  <si>
+    <t>https://www.smarttask.io/</t>
+  </si>
+  <si>
+    <t>smarttask.io/</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,17 +102,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,63 +448,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.69921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Url</v>
-      </c>
-      <c r="B1" t="str">
-        <v>WebsiteName</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>https://www.needingadvice.co.uk/</v>
-      </c>
-      <c r="B2" t="str">
-        <v>needingadvice_co_uk</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>https://plurality.network/</v>
-      </c>
-      <c r="B3" t="str">
-        <v>plurality_network</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>https://rateswitchrewards.co.uk/</v>
-      </c>
-      <c r="B4" t="str">
-        <v>rateswitchrewards_co_uk</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>http://samantus.com/</v>
-      </c>
-      <c r="B5" t="str">
-        <v>samantus_com</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>https://www.schoolofpodcasting.com/</v>
-      </c>
-      <c r="B6" t="str">
-        <v>schoolofpodcasting_com</v>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" xr:uid="{8C37CE58-606B-4132-9FAF-227C6DD2B082}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
+    <ignoredError sqref="A1:B6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>